<commit_message>
corrección de errores menores
numeración correcta de m101
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/escaleta CN_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/escaleta CN_08_02_CO.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="236">
   <si>
     <t>Asignatura</t>
   </si>
@@ -721,6 +721,12 @@
   </si>
   <si>
     <t>Recurso M102AB-02</t>
+  </si>
+  <si>
+    <t>Recurso M101A-03</t>
+  </si>
+  <si>
+    <t>Recurso M101A-04</t>
   </si>
 </sst>
 </file>
@@ -932,34 +938,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -999,6 +987,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1307,9 +1313,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U290"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,94 +1343,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="22" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="25" t="s">
+      <c r="N1" s="39"/>
+      <c r="O1" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="T1" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="42" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="22" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="40"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="23" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2195,7 +2201,7 @@
         <v>196</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>198</v>
@@ -2492,7 +2498,7 @@
         <v>196</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="U20" s="10" t="s">
         <v>198</v>
@@ -4314,6 +4320,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4328,12 +4340,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>